<commit_message>
* manual algorithm test (non source)
</commit_message>
<xml_diff>
--- a/src/test/resources/kuhviertel/h_values.xlsx
+++ b/src/test/resources/kuhviertel/h_values.xlsx
@@ -3,23 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrissW-R1\Desktop\kuhviertel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="7470" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Edges" sheetId="3" r:id="rId2"/>
     <sheet name="Links" sheetId="2" r:id="rId3"/>
+    <sheet name="OpenList" sheetId="4" r:id="rId4"/>
+    <sheet name="ClosedList" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Nodes!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ClosedList!$A$1:$A$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Edges!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Links!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Nodes!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OpenList!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:P22"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -48,13 +50,34 @@
   <si>
     <t>h_Finish</t>
   </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>tentative_g:</t>
+  </si>
+  <si>
+    <t>currentNode:</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>predecessor</t>
+  </si>
+  <si>
+    <t>f:</t>
+  </si>
+  <si>
+    <t>successor:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,17 +110,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,20 +398,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -398,8 +423,14 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -409,8 +440,11 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -420,8 +454,14 @@
       <c r="C3" s="1">
         <v>29.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -431,8 +471,14 @@
       <c r="C4" s="1">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>66.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -443,7 +489,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -454,7 +500,7 @@
         <v>123.2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -465,7 +511,7 @@
         <v>160.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -476,7 +522,7 @@
         <v>206.7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -487,7 +533,7 @@
         <v>310.10000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -498,7 +544,7 @@
         <v>355.2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -509,7 +555,7 @@
         <v>88.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -520,7 +566,7 @@
         <v>93.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -531,7 +577,7 @@
         <v>157.19999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -542,7 +588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -553,7 +599,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -564,7 +610,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -575,7 +621,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -586,7 +632,7 @@
         <v>240.9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -597,7 +643,7 @@
         <v>287.3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -608,7 +654,7 @@
         <v>328.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -619,7 +665,7 @@
         <v>314.89999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -630,7 +676,7 @@
         <v>340.8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -641,7 +687,7 @@
         <v>362.8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -652,7 +698,7 @@
         <v>368.4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -663,7 +709,7 @@
         <v>386.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -674,7 +720,7 @@
         <v>401.2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -685,7 +731,7 @@
         <v>404.8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -696,7 +742,7 @@
         <v>425.1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -707,7 +753,7 @@
         <v>429.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -718,7 +764,7 @@
         <v>487.8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -729,7 +775,7 @@
         <v>482.3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -740,7 +786,7 @@
         <v>474.3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -751,7 +797,7 @@
         <v>468.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -762,7 +808,7 @@
         <v>466.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -773,7 +819,7 @@
         <v>474.4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -784,7 +830,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -795,7 +841,7 @@
         <v>271.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -806,7 +852,7 @@
         <v>311.2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -817,7 +863,7 @@
         <v>326.3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -828,7 +874,7 @@
         <v>338.1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -839,7 +885,7 @@
         <v>364.3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -850,7 +896,7 @@
         <v>370.4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -861,7 +907,7 @@
         <v>377.4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -872,7 +918,7 @@
         <v>382.1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -883,7 +929,7 @@
         <v>404.6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -894,7 +940,7 @@
         <v>411.9</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -904,8 +950,14 @@
       <c r="C47" s="1">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -915,8 +967,14 @@
       <c r="C48" s="1">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>46</v>
+      </c>
+      <c r="E48" s="1">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -926,8 +984,14 @@
       <c r="C49" s="1">
         <v>44.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>47</v>
+      </c>
+      <c r="E49" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -937,8 +1001,14 @@
       <c r="C50" s="1">
         <v>60.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -949,7 +1019,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -960,7 +1030,7 @@
         <v>197.7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -971,7 +1041,7 @@
         <v>280.60000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -982,7 +1052,7 @@
         <v>342.1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -993,7 +1063,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1004,7 +1074,7 @@
         <v>398.4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1015,7 +1085,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1026,7 +1096,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1037,7 +1107,7 @@
         <v>47.8</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1048,7 +1118,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>61</v>
       </c>
@@ -1059,7 +1129,7 @@
         <v>173.3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62</v>
       </c>
@@ -1070,7 +1140,7 @@
         <v>215.3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
       </c>
@@ -1081,7 +1151,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>64</v>
       </c>
@@ -1092,7 +1162,7 @@
         <v>358.7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
@@ -1103,7 +1173,7 @@
         <v>392.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
@@ -1114,7 +1184,7 @@
         <v>429.9</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
@@ -1125,7 +1195,7 @@
         <v>444.7</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
@@ -1136,7 +1206,7 @@
         <v>454.5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
@@ -1147,7 +1217,7 @@
         <v>495.6</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
@@ -1158,7 +1228,7 @@
         <v>510.6</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
@@ -1169,7 +1239,7 @@
         <v>530.20000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
@@ -1180,7 +1250,7 @@
         <v>217.2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
@@ -1192,7 +1262,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:E1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1201,25 +1271,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2429,6 +2499,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1">
+    <filterColumn colId="1" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -2440,13 +2513,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2454,12 +2527,12 @@
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3338,9 +3411,139 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1">
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1">
+        <v>547.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>540.20000000000005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <f>Nodes!E50+Edges!D43</f>
+        <v>88.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <f>E3+Nodes!B49</f>
+        <v>577.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="A1:B1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ added new handler, which connects to the Overpass API + added sample implementation of the A* alogrithm * marked OsmHandler06 as deprecated * corrected Kuhviertel test data
</commit_message>
<xml_diff>
--- a/src/test/resources/kuhviertel/h_values.xlsx
+++ b/src/test/resources/kuhviertel/h_values.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrissW-R1\workspace\ParRoute\src\test\resources\kuhviertel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="7470" activeTab="3"/>
   </bookViews>
@@ -21,7 +26,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OpenList!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:P22"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +124,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,7 +408,7 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -610,7 +614,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -621,7 +625,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -632,7 +636,7 @@
         <v>240.9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -643,7 +647,7 @@
         <v>287.3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -654,7 +658,7 @@
         <v>328.8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -665,7 +669,7 @@
         <v>314.89999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -676,7 +680,7 @@
         <v>340.8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -687,7 +691,7 @@
         <v>362.8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -698,7 +702,7 @@
         <v>368.4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -709,7 +713,7 @@
         <v>386.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -720,7 +724,7 @@
         <v>401.2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -731,7 +735,7 @@
         <v>404.8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -742,7 +746,7 @@
         <v>425.1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -753,7 +757,7 @@
         <v>429.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -764,7 +768,7 @@
         <v>487.8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -775,7 +779,7 @@
         <v>482.3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1162,7 +1166,7 @@
         <v>358.7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>65</v>
       </c>
@@ -1173,7 +1177,7 @@
         <v>392.5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>66</v>
       </c>
@@ -1184,7 +1188,7 @@
         <v>429.9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
@@ -1195,7 +1199,7 @@
         <v>444.7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>454.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
@@ -1217,7 +1221,7 @@
         <v>495.6</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
@@ -1228,7 +1232,7 @@
         <v>510.6</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>71</v>
       </c>
@@ -1239,7 +1243,7 @@
         <v>530.20000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>72</v>
       </c>
@@ -1250,7 +1254,7 @@
         <v>217.2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
@@ -1271,11 +1275,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.7109375" customWidth="1"/>
@@ -2478,7 +2482,7 @@
         <v>25</v>
       </c>
       <c r="C86">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D86" s="1">
         <v>50.8</v>
@@ -2513,11 +2517,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="5.7109375" customWidth="1"/>
@@ -2720,7 +2724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2734,7 +2738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2759,7 +2763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2798,7 +2802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2809,7 +2813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2823,7 +2827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2831,16 +2835,13 @@
         <v>65</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D25">
-        <v>64</v>
-      </c>
-      <c r="E25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3299,7 +3300,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C64">
         <v>63</v>
@@ -3425,13 +3426,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -3491,7 +3492,6 @@
         <v>577.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:B1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3501,43 +3501,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>48</v>
       </c>

</xml_diff>